<commit_message>
Revert to simplified BasePage structure and fix unused variables
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -35,10 +35,10 @@
     <t>siteUrl</t>
   </si>
   <si>
-    <t>BaseUrl</t>
-  </si>
-  <si>
-    <t>autosuggest query</t>
+    <t>baseUrl</t>
+  </si>
+  <si>
+    <t>autosuggest</t>
   </si>
   <si>
     <t>autosuggestEndpoint</t>
@@ -47,7 +47,7 @@
     <t>query</t>
   </si>
   <si>
-    <t>search query</t>
+    <t>search</t>
   </si>
   <si>
     <t>searchEndpoint</t>
@@ -83,13 +83,13 @@
     <t>https://www.footlocker.my/</t>
   </si>
   <si>
-    <t>https://search.unbxd.io/7018997f7a60dcb95e1eec824707326b/ss-unbxd-aapac-prod-mapactive-en-SG65121748367149/</t>
+    <t>https://search.unbxd.io/6d50ad03aeb54e49824ed69599611106/ss-unbxd-aapac-prod-mapactive-en-MY65121748366945/</t>
   </si>
   <si>
     <t>&amp;inFields.count=0&amp;topQueries.count=4&amp;keywordSuggestions.count=4&amp;popularProducts.count=4&amp;promotedSuggestion.count=5&amp;indent=off&amp;popularProducts.fields=doctype,imageUrl,title,doctype,autosuggest,price,imageUrl,productUrl,autosuggest</t>
   </si>
   <si>
-    <t>jordan</t>
+    <t>puma shoes</t>
   </si>
   <si>
     <t>mwave</t>
@@ -808,13 +808,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1293,10 +1294,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E$1:E$1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="36" customHeight="1"/>
@@ -1332,208 +1333,231 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:7">
-      <c r="A2" s="3" t="s">
+    <row r="2" customHeight="1" spans="1:9">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
-    <row r="3" customHeight="1" spans="1:7">
-      <c r="A3" s="3" t="s">
+    <row r="3" customHeight="1" spans="1:9">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" customHeight="1" spans="1:9">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:7">
-      <c r="A5" s="3" t="s">
+    <row r="5" customHeight="1" spans="1:9">
+      <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
-    <row r="6" customHeight="1" spans="1:7">
-      <c r="A6" s="3" t="s">
+    <row r="6" customHeight="1" spans="1:9">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
-    <row r="7" customHeight="1" spans="1:7">
-      <c r="A7" s="3" t="s">
+    <row r="7" customHeight="1" spans="1:9">
+      <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
-    <row r="8" customHeight="1" spans="1:7">
-      <c r="A8" s="3" t="s">
+    <row r="8" customHeight="1" spans="1:9">
+      <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" customHeight="1" spans="1:9">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9"/>
-      <c r="F9" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>50</v>
       </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:9">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://www.shoppersstop.com/" tooltip="https://www.shoppersstop.com/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://www.footlocker.my/" tooltip="https://www.footlocker.my/"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://search.unbxd.io/7018997f7a60dcb95e1eec824707326b/ss-unbxd-aapac-prod-mapactive-en-SG65121748367149/" tooltip="https://search.unbxd.io/7018997f7a60dcb95e1eec824707326b/ss-unbxd-aapac-prod-mapactive-en-SG65121748367149/"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://search.unbxd.io/6d50ad03aeb54e49824ed69599611106/ss-unbxd-aapac-prod-mapactive-en-MY65121748366945/" tooltip="https://search.unbxd.io/6d50ad03aeb54e49824ed69599611106/ss-unbxd-aapac-prod-mapactive-en-MY65121748366945/"/>
     <hyperlink ref="B4" r:id="rId4" display="https://www.mwave.com.au/" tooltip="https://www.mwave.com.au/"/>
     <hyperlink ref="C4" r:id="rId5" display="https://search.unbxd.io/0de1e06bc0d3f62b42fb175e361758af/ss-unbxd-prod-mwave43601693203163/" tooltip="https://search.unbxd.io/0de1e06bc0d3f62b42fb175e361758af/ss-unbxd-prod-mwave43601693203163/"/>
     <hyperlink ref="B5" r:id="rId6" display="https://www.durian.in/" tooltip="https://www.durian.in/"/>

</xml_diff>